<commit_message>
Test env updates for verifying algorithm and input validation fixes
</commit_message>
<xml_diff>
--- a/test_data/by_number/p_td_1_non_full.xlsx
+++ b/test_data/by_number/p_td_1_non_full.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lonnychen/Dropbox/@project - HERTIE SCHOOL/MDS/COURSES/Spring 2024/Data Structures &amp; Algorithms (C9)/Project/student-project-matching/test_data/by_matching/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lonnychen/Dropbox/@project - HERTIE SCHOOL/MDS/COURSES/Spring 2024/Data Structures &amp; Algorithms (C9)/Project/student-project-matching/test_data/by_number/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D1D0629-BB8D-F54A-860D-2A8A1DE5BC18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69DE23F0-0EFB-174B-8DB4-3509D1594AC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7380" yWindow="6880" windowWidth="28040" windowHeight="16560" xr2:uid="{167CAB08-E6E9-D544-8315-BD75E8338A04}"/>
+    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16560" xr2:uid="{167CAB08-E6E9-D544-8315-BD75E8338A04}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -447,7 +447,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -495,10 +495,10 @@
         <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -509,19 +509,19 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -532,19 +532,19 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>